<commit_message>
Filled out Board and BoardCell classes to pass tests, added BadConfigFormatException to detect bad config files
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameNANS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Senior Year\Software\Workspace\ClueGameNANS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="Y24" sqref="A1:Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,9 +612,7 @@
       <c r="Y1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="1">
-        <v>0</v>
-      </c>
+      <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -692,10 +690,7 @@
       <c r="Y2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="1">
-        <f>Z1+1</f>
-        <v>1</v>
-      </c>
+      <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -773,10 +768,7 @@
       <c r="Y3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="1">
-        <f t="shared" ref="Z3:Z24" si="0">Z2+1</f>
-        <v>2</v>
-      </c>
+      <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -854,10 +846,7 @@
       <c r="Y4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -935,10 +924,7 @@
       <c r="Y5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+      <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1016,10 +1002,7 @@
       <c r="Y6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z6" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1097,10 +1080,7 @@
       <c r="Y7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
+      <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1178,10 +1158,7 @@
       <c r="Y8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
+      <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1259,10 +1236,7 @@
       <c r="Y9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z9" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
+      <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1340,10 +1314,7 @@
       <c r="Y10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z10" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
+      <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1421,10 +1392,7 @@
       <c r="Y11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z11" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1502,10 +1470,7 @@
       <c r="Y12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Z12" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
+      <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1583,10 +1548,7 @@
       <c r="Y13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z13" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
+      <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1664,10 +1626,7 @@
       <c r="Y14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z14" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
+      <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1745,10 +1704,7 @@
       <c r="Y15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z15" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
+      <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1826,10 +1782,7 @@
       <c r="Y16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z16" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+      <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1907,10 +1860,7 @@
       <c r="Y17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z17" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1988,10 +1938,7 @@
       <c r="Y18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z18" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -2069,10 +2016,7 @@
       <c r="Y19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z19" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
+      <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -2150,10 +2094,7 @@
       <c r="Y20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z20" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
+      <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -2231,10 +2172,7 @@
       <c r="Y21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z21" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+      <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2312,10 +2250,7 @@
       <c r="Y22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z22" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
+      <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -2393,10 +2328,7 @@
       <c r="Y23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z23" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
+      <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -2474,111 +2406,34 @@
       <c r="Y24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Z24" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
+      <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <v>0</v>
-      </c>
-      <c r="B25" s="13">
-        <f>A25+1</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="13">
-        <f t="shared" ref="C25:Y25" si="1">B25+1</f>
-        <v>2</v>
-      </c>
-      <c r="D25" s="13">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E25" s="13">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F25" s="13">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G25" s="13">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H25" s="13">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="I25" s="13">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="J25" s="13">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="K25" s="13">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L25" s="13">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="M25" s="13">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="N25" s="13">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="O25" s="13">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="P25" s="13">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="Q25" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="R25" s="13">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="S25" s="13">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="T25" s="13">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="U25" s="13">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="V25" s="13">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="W25" s="13">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="X25" s="13">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="Y25" s="13">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
     </row>
     <row r="26" spans="1:26" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>

</xml_diff>